<commit_message>
1008113 - X12 Specifications 850 and 855 - Updated specifications with Customer Release Number
</commit_message>
<xml_diff>
--- a/format-specifications/ansi-x12/4010/855/Pagero-ANSI-X12-4010-855-ordrsp-description-outbound.xlsx
+++ b/format-specifications/ansi-x12/4010/855/Pagero-ANSI-X12-4010-855-ordrsp-description-outbound.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\format\paysol-transformation\templates\X12\ordrsp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CEAD11-2C39-4296-AB0F-0EE711FF0C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7790FCB5-3CBC-474D-AC60-4FBCA1D899F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="5010" windowWidth="24570" windowHeight="16320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="1260" windowWidth="38700" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -1158,6 +1158,9 @@
     <t>ST*855*123456789~</t>
   </si>
   <si>
+    <t>850</t>
+  </si>
+  <si>
     <t>01 if numeric 9 token ZZ otherwise</t>
   </si>
   <si>
@@ -1334,9 +1337,6 @@
   </si>
   <si>
     <t xml:space="preserve">Used as Buyer order row number if no REF*BV is sent </t>
-  </si>
-  <si>
-    <t>855</t>
   </si>
 </sst>
 </file>
@@ -1930,14 +1930,46 @@
     <xf numFmtId="49" fontId="11" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -1946,39 +1978,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2415,7 +2415,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="2"/>
@@ -2490,7 +2490,7 @@
     <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="94" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C10" s="95"/>
       <c r="D10" s="96"/>
@@ -2601,10 +2601,10 @@
         <v>44978</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E24" s="2"/>
     </row>
@@ -2709,8 +2709,8 @@
   <dimension ref="A1:H167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G110" sqref="G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2758,7 +2758,7 @@
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="31" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2882,7 +2882,7 @@
         <v>322</v>
       </c>
       <c r="G8" s="38" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2928,7 +2928,7 @@
         <v>322</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3132,21 +3132,21 @@
         <v>332</v>
       </c>
       <c r="G19" s="38" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B20" s="107" t="s">
+      <c r="B20" s="116" t="s">
         <v>362</v>
       </c>
-      <c r="C20" s="108"/>
-      <c r="D20" s="108"/>
-      <c r="E20" s="108"/>
-      <c r="F20" s="108"/>
-      <c r="G20" s="108"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="117"/>
+      <c r="G20" s="117"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="38"/>
@@ -3355,14 +3355,14 @@
       <c r="A31" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B31" s="109" t="s">
+      <c r="B31" s="104" t="s">
         <v>336</v>
       </c>
-      <c r="C31" s="110"/>
-      <c r="D31" s="110"/>
-      <c r="E31" s="110"/>
-      <c r="F31" s="110"/>
-      <c r="G31" s="111"/>
+      <c r="C31" s="108"/>
+      <c r="D31" s="108"/>
+      <c r="E31" s="108"/>
+      <c r="F31" s="108"/>
+      <c r="G31" s="118"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="45"/>
@@ -3405,7 +3405,7 @@
         <v>109</v>
       </c>
       <c r="F34" s="41" t="s">
-        <v>426</v>
+        <v>369</v>
       </c>
       <c r="G34" s="38" t="s">
         <v>248</v>
@@ -3438,14 +3438,14 @@
       <c r="A36" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B36" s="109" t="s">
+      <c r="B36" s="104" t="s">
         <v>368</v>
       </c>
-      <c r="C36" s="110"/>
-      <c r="D36" s="110"/>
-      <c r="E36" s="110"/>
-      <c r="F36" s="110"/>
-      <c r="G36" s="111"/>
+      <c r="C36" s="108"/>
+      <c r="D36" s="108"/>
+      <c r="E36" s="108"/>
+      <c r="F36" s="108"/>
+      <c r="G36" s="118"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="38"/>
@@ -3511,10 +3511,10 @@
         <v>29</v>
       </c>
       <c r="F40" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="G40" s="38" t="s">
         <v>374</v>
-      </c>
-      <c r="G40" s="38" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -3534,10 +3534,10 @@
         <v>117</v>
       </c>
       <c r="F41" s="41" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="G41" s="38" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
@@ -3580,7 +3580,7 @@
         <v>119</v>
       </c>
       <c r="F43" s="41" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="G43" s="38"/>
     </row>
@@ -3601,7 +3601,7 @@
         <v>92</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="G44" s="38" t="s">
         <v>218</v>
@@ -3611,14 +3611,14 @@
       <c r="A45" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B45" s="109" t="s">
-        <v>371</v>
-      </c>
-      <c r="C45" s="110"/>
-      <c r="D45" s="110"/>
-      <c r="E45" s="110"/>
-      <c r="F45" s="110"/>
-      <c r="G45" s="111"/>
+      <c r="B45" s="104" t="s">
+        <v>372</v>
+      </c>
+      <c r="C45" s="108"/>
+      <c r="D45" s="108"/>
+      <c r="E45" s="108"/>
+      <c r="F45" s="108"/>
+      <c r="G45" s="118"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="38"/>
@@ -3886,7 +3886,7 @@
         <v>109</v>
       </c>
       <c r="F61" s="41" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G61" s="38" t="s">
         <v>256</v>
@@ -3909,7 +3909,7 @@
         <v>92</v>
       </c>
       <c r="F62" s="41" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="G62" s="38" t="s">
         <v>93</v>
@@ -3919,8 +3919,8 @@
       <c r="A63" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B63" s="109" t="s">
-        <v>377</v>
+      <c r="B63" s="104" t="s">
+        <v>378</v>
       </c>
       <c r="C63" s="105"/>
       <c r="D63" s="105"/>
@@ -3965,7 +3965,7 @@
         <v>109</v>
       </c>
       <c r="F66" s="41" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G66" s="38" t="s">
         <v>272</v>
@@ -3988,7 +3988,7 @@
         <v>92</v>
       </c>
       <c r="F67" s="41" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="G67" s="38" t="s">
         <v>93</v>
@@ -3998,7 +3998,7 @@
       <c r="A68" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B68" s="109" t="s">
+      <c r="B68" s="104" t="s">
         <v>341</v>
       </c>
       <c r="C68" s="105"/>
@@ -4046,7 +4046,7 @@
         <v>120</v>
       </c>
       <c r="F71" s="41" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="G71" s="68" t="s">
         <v>230</v>
@@ -4067,7 +4067,7 @@
         <v>119</v>
       </c>
       <c r="F72" s="41" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="G72" s="69" t="s">
         <v>307</v>
@@ -4099,7 +4099,7 @@
         <v>234</v>
       </c>
       <c r="F74" s="41" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="G74" s="68"/>
     </row>
@@ -4107,7 +4107,7 @@
       <c r="A75" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B75" s="109" t="s">
+      <c r="B75" s="104" t="s">
         <v>342</v>
       </c>
       <c r="C75" s="105"/>
@@ -4191,7 +4191,7 @@
         <v>123</v>
       </c>
       <c r="F80" s="41" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G80" s="38"/>
     </row>
@@ -4212,7 +4212,7 @@
         <v>101</v>
       </c>
       <c r="F81" s="41" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G81" s="38" t="s">
         <v>306</v>
@@ -4235,7 +4235,7 @@
         <v>134</v>
       </c>
       <c r="F82" s="70" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="G82" s="51" t="s">
         <v>224</v>
@@ -4282,7 +4282,7 @@
         <v>123</v>
       </c>
       <c r="F85" s="41" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G85" s="38" t="s">
         <v>273</v>
@@ -4318,7 +4318,7 @@
         <v>141</v>
       </c>
       <c r="F87" s="52" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G87" s="51" t="s">
         <v>224</v>
@@ -4369,7 +4369,7 @@
         <v>145</v>
       </c>
       <c r="F90" s="41" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="G90" s="38"/>
     </row>
@@ -4390,7 +4390,7 @@
         <v>29</v>
       </c>
       <c r="F91" s="41" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="G91" s="38"/>
     </row>
@@ -4411,7 +4411,7 @@
         <v>149</v>
       </c>
       <c r="F92" s="41" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="G92" s="38"/>
     </row>
@@ -4432,7 +4432,7 @@
         <v>120</v>
       </c>
       <c r="F93" s="41" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="G93" s="38"/>
     </row>
@@ -4440,7 +4440,7 @@
       <c r="A94" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B94" s="104" t="s">
+      <c r="B94" s="112" t="s">
         <v>344</v>
       </c>
       <c r="C94" s="105"/>
@@ -4451,7 +4451,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="38"/>
-      <c r="B95" s="104" t="s">
+      <c r="B95" s="112" t="s">
         <v>345</v>
       </c>
       <c r="C95" s="105"/>
@@ -4462,7 +4462,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="38"/>
-      <c r="B96" s="104" t="s">
+      <c r="B96" s="112" t="s">
         <v>346</v>
       </c>
       <c r="C96" s="105"/>
@@ -4473,7 +4473,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="38"/>
-      <c r="B97" s="104" t="s">
+      <c r="B97" s="112" t="s">
         <v>347</v>
       </c>
       <c r="C97" s="105"/>
@@ -4484,7 +4484,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="38"/>
-      <c r="B98" s="104" t="s">
+      <c r="B98" s="112" t="s">
         <v>348</v>
       </c>
       <c r="C98" s="105"/>
@@ -4495,7 +4495,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="38"/>
-      <c r="B99" s="104" t="s">
+      <c r="B99" s="112" t="s">
         <v>345</v>
       </c>
       <c r="C99" s="105"/>
@@ -4506,7 +4506,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="38"/>
-      <c r="B100" s="104" t="s">
+      <c r="B100" s="112" t="s">
         <v>349</v>
       </c>
       <c r="C100" s="105"/>
@@ -4517,7 +4517,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="38"/>
-      <c r="B101" s="104" t="s">
+      <c r="B101" s="112" t="s">
         <v>350</v>
       </c>
       <c r="C101" s="105"/>
@@ -4528,7 +4528,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="38"/>
-      <c r="B102" s="104" t="s">
+      <c r="B102" s="112" t="s">
         <v>351</v>
       </c>
       <c r="C102" s="105"/>
@@ -4539,36 +4539,36 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="38"/>
-      <c r="B103" s="109" t="s">
+      <c r="B103" s="104" t="s">
         <v>345</v>
       </c>
-      <c r="C103" s="112"/>
-      <c r="D103" s="112"/>
-      <c r="E103" s="112"/>
-      <c r="F103" s="112"/>
-      <c r="G103" s="113"/>
+      <c r="C103" s="113"/>
+      <c r="D103" s="113"/>
+      <c r="E103" s="113"/>
+      <c r="F103" s="113"/>
+      <c r="G103" s="114"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="38"/>
-      <c r="B104" s="109" t="s">
+      <c r="B104" s="104" t="s">
         <v>352</v>
       </c>
-      <c r="C104" s="112"/>
-      <c r="D104" s="112"/>
-      <c r="E104" s="112"/>
-      <c r="F104" s="112"/>
-      <c r="G104" s="113"/>
+      <c r="C104" s="113"/>
+      <c r="D104" s="113"/>
+      <c r="E104" s="113"/>
+      <c r="F104" s="113"/>
+      <c r="G104" s="114"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="38"/>
-      <c r="B105" s="109" t="s">
+      <c r="B105" s="104" t="s">
         <v>353</v>
       </c>
-      <c r="C105" s="112"/>
-      <c r="D105" s="112"/>
-      <c r="E105" s="112"/>
-      <c r="F105" s="112"/>
-      <c r="G105" s="113"/>
+      <c r="C105" s="113"/>
+      <c r="D105" s="113"/>
+      <c r="E105" s="113"/>
+      <c r="F105" s="113"/>
+      <c r="G105" s="114"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="38"/>
@@ -4632,7 +4632,7 @@
         <v>309</v>
       </c>
       <c r="G110" s="43" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
@@ -4863,7 +4863,7 @@
       <c r="A121" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B121" s="114" t="s">
+      <c r="B121" s="107" t="s">
         <v>319</v>
       </c>
       <c r="C121" s="115"/>
@@ -4912,7 +4912,7 @@
         <v>64</v>
       </c>
       <c r="F124" s="41" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="G124" s="43" t="s">
         <v>244</v>
@@ -4998,7 +4998,7 @@
         <v>124</v>
       </c>
       <c r="F128" s="41" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G128" s="43" t="s">
         <v>22</v>
@@ -5008,14 +5008,14 @@
       <c r="A129" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B129" s="114" t="s">
-        <v>394</v>
-      </c>
-      <c r="C129" s="110"/>
-      <c r="D129" s="110"/>
-      <c r="E129" s="110"/>
-      <c r="F129" s="110"/>
-      <c r="G129" s="110"/>
+      <c r="B129" s="107" t="s">
+        <v>395</v>
+      </c>
+      <c r="C129" s="108"/>
+      <c r="D129" s="108"/>
+      <c r="E129" s="108"/>
+      <c r="F129" s="108"/>
+      <c r="G129" s="108"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="43"/>
@@ -5028,7 +5028,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="35" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B131" s="35"/>
       <c r="C131" s="35"/>
@@ -5039,30 +5039,30 @@
     </row>
     <row r="132" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A132" s="85" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B132" s="86">
         <v>128</v>
       </c>
       <c r="C132" s="86" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D132" s="85" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E132" s="86" t="s">
         <v>120</v>
       </c>
       <c r="F132" s="86" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G132" s="87" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A133" s="85" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B133" s="86">
         <v>127</v>
@@ -5074,21 +5074,21 @@
         <v>122</v>
       </c>
       <c r="E133" s="86" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F133" s="86" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="G133" s="87" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B134" s="109" t="s">
-        <v>419</v>
+      <c r="B134" s="104" t="s">
+        <v>420</v>
       </c>
       <c r="C134" s="105"/>
       <c r="D134" s="105"/>
@@ -5107,7 +5107,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="35" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B136" s="35"/>
       <c r="C136" s="35"/>
@@ -5118,30 +5118,30 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="85" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B137" s="86">
         <v>128</v>
       </c>
       <c r="C137" s="86" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D137" s="87" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E137" s="87" t="s">
         <v>120</v>
       </c>
       <c r="F137" s="87" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G137" s="87" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A138" s="85" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B138" s="86">
         <v>127</v>
@@ -5153,21 +5153,21 @@
         <v>122</v>
       </c>
       <c r="E138" s="87" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F138" s="87" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="G138" s="87" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B139" s="109" t="s">
-        <v>424</v>
+      <c r="B139" s="104" t="s">
+        <v>425</v>
       </c>
       <c r="C139" s="105"/>
       <c r="D139" s="105"/>
@@ -5212,7 +5212,7 @@
         <v>29</v>
       </c>
       <c r="F142" s="41" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G142" s="68" t="s">
         <v>334</v>
@@ -5233,7 +5233,7 @@
         <v>159</v>
       </c>
       <c r="F143" s="41" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="G143" s="69"/>
     </row>
@@ -5273,7 +5273,7 @@
         <v>234</v>
       </c>
       <c r="F145" s="41" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G145" s="68" t="s">
         <v>265</v>
@@ -5294,7 +5294,7 @@
         <v>234</v>
       </c>
       <c r="F146" s="41" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="G146" s="68"/>
     </row>
@@ -5302,14 +5302,14 @@
       <c r="A147" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B147" s="114" t="s">
+      <c r="B147" s="107" t="s">
         <v>354</v>
       </c>
-      <c r="C147" s="110"/>
-      <c r="D147" s="110"/>
-      <c r="E147" s="110"/>
-      <c r="F147" s="110"/>
-      <c r="G147" s="110"/>
+      <c r="C147" s="108"/>
+      <c r="D147" s="108"/>
+      <c r="E147" s="108"/>
+      <c r="F147" s="108"/>
+      <c r="G147" s="108"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="45"/>
@@ -5373,14 +5373,14 @@
       <c r="A152" s="78" t="s">
         <v>301</v>
       </c>
-      <c r="B152" s="116" t="s">
+      <c r="B152" s="109" t="s">
         <v>355</v>
       </c>
-      <c r="C152" s="117"/>
-      <c r="D152" s="117"/>
-      <c r="E152" s="117"/>
-      <c r="F152" s="117"/>
-      <c r="G152" s="118"/>
+      <c r="C152" s="110"/>
+      <c r="D152" s="110"/>
+      <c r="E152" s="110"/>
+      <c r="F152" s="110"/>
+      <c r="G152" s="111"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="43"/>
@@ -5423,7 +5423,7 @@
         <v>173</v>
       </c>
       <c r="F155" s="41" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G155" s="43" t="s">
         <v>246</v>
@@ -5456,8 +5456,8 @@
       <c r="A157" s="78" t="s">
         <v>301</v>
       </c>
-      <c r="B157" s="104" t="s">
-        <v>402</v>
+      <c r="B157" s="112" t="s">
+        <v>403</v>
       </c>
       <c r="C157" s="105"/>
       <c r="D157" s="105"/>
@@ -5535,14 +5535,14 @@
       <c r="A162" s="78" t="s">
         <v>301</v>
       </c>
-      <c r="B162" s="109" t="s">
-        <v>400</v>
-      </c>
-      <c r="C162" s="112"/>
-      <c r="D162" s="112"/>
-      <c r="E162" s="112"/>
-      <c r="F162" s="112"/>
-      <c r="G162" s="113"/>
+      <c r="B162" s="104" t="s">
+        <v>401</v>
+      </c>
+      <c r="C162" s="113"/>
+      <c r="D162" s="113"/>
+      <c r="E162" s="113"/>
+      <c r="F162" s="113"/>
+      <c r="G162" s="114"/>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="78"/>
@@ -5618,32 +5618,17 @@
       <c r="A167" s="78" t="s">
         <v>301</v>
       </c>
-      <c r="B167" s="109" t="s">
-        <v>401</v>
-      </c>
-      <c r="C167" s="112"/>
-      <c r="D167" s="112"/>
-      <c r="E167" s="112"/>
-      <c r="F167" s="112"/>
-      <c r="G167" s="113"/>
+      <c r="B167" s="104" t="s">
+        <v>402</v>
+      </c>
+      <c r="C167" s="113"/>
+      <c r="D167" s="113"/>
+      <c r="E167" s="113"/>
+      <c r="F167" s="113"/>
+      <c r="G167" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B162:G162"/>
-    <mergeCell ref="B167:G167"/>
-    <mergeCell ref="B105:G105"/>
-    <mergeCell ref="B121:G121"/>
-    <mergeCell ref="B129:G129"/>
-    <mergeCell ref="B134:G134"/>
-    <mergeCell ref="B139:G139"/>
-    <mergeCell ref="B147:G147"/>
-    <mergeCell ref="B152:G152"/>
-    <mergeCell ref="B157:G157"/>
-    <mergeCell ref="B100:G100"/>
-    <mergeCell ref="B101:G101"/>
-    <mergeCell ref="B102:G102"/>
-    <mergeCell ref="B103:G103"/>
-    <mergeCell ref="B104:G104"/>
     <mergeCell ref="B99:G99"/>
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="B31:G31"/>
@@ -5657,6 +5642,21 @@
     <mergeCell ref="B96:G96"/>
     <mergeCell ref="B97:G97"/>
     <mergeCell ref="B98:G98"/>
+    <mergeCell ref="B100:G100"/>
+    <mergeCell ref="B101:G101"/>
+    <mergeCell ref="B102:G102"/>
+    <mergeCell ref="B103:G103"/>
+    <mergeCell ref="B104:G104"/>
+    <mergeCell ref="B162:G162"/>
+    <mergeCell ref="B167:G167"/>
+    <mergeCell ref="B105:G105"/>
+    <mergeCell ref="B121:G121"/>
+    <mergeCell ref="B129:G129"/>
+    <mergeCell ref="B134:G134"/>
+    <mergeCell ref="B139:G139"/>
+    <mergeCell ref="B147:G147"/>
+    <mergeCell ref="B152:G152"/>
+    <mergeCell ref="B157:G157"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5795,7 +5795,7 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="83" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
@@ -5810,17 +5810,17 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="83" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="83" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="84" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -5959,7 +5959,7 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="83" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
@@ -5974,17 +5974,17 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="83" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="83" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="84" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -6123,7 +6123,7 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="83" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
@@ -6138,17 +6138,17 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="83" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="83" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="84" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -6291,52 +6291,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <of481e2e1c3c48d48da92bf63b539923 xmlns="cb09451c-b582-4d10-a9a3-b0b7d3fa26c8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Delivery</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6b8c302d-7163-4ebf-92ca-9cf30af76f8d</TermId>
-        </TermInfo>
-      </Terms>
-    </of481e2e1c3c48d48da92bf63b539923>
-    <Document_x0020_Classification xmlns="cb09451c-b582-4d10-a9a3-b0b7d3fa26c8">Internal</Document_x0020_Classification>
-    <Responsible xmlns="cb09451c-b582-4d10-a9a3-b0b7d3fa26c8">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Responsible>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Document_x0020_Owner xmlns="cb09451c-b582-4d10-a9a3-b0b7d3fa26c8">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Document_x0020_Owner>
-    <TaxCatchAll xmlns="bf46d841-c562-4023-88f4-20dc8ac77732">
-      <Value>16</Value>
-    </TaxCatchAll>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E7CAF200281DA4BB762244EA838702E" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ec206a3de9ab8848ad5fbf6dc651eca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="cb09451c-b582-4d10-a9a3-b0b7d3fa26c8" xmlns:ns3="bf46d841-c562-4023-88f4-20dc8ac77732" xmlns:ns4="966ee308-7f72-40a1-8e25-c38950f75702" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="17cf1002c781355239d92ae5c7c8c75e" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6653,10 +6607,69 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <of481e2e1c3c48d48da92bf63b539923 xmlns="cb09451c-b582-4d10-a9a3-b0b7d3fa26c8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Delivery</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6b8c302d-7163-4ebf-92ca-9cf30af76f8d</TermId>
+        </TermInfo>
+      </Terms>
+    </of481e2e1c3c48d48da92bf63b539923>
+    <Document_x0020_Classification xmlns="cb09451c-b582-4d10-a9a3-b0b7d3fa26c8">Internal</Document_x0020_Classification>
+    <Responsible xmlns="cb09451c-b582-4d10-a9a3-b0b7d3fa26c8">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Responsible>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Document_x0020_Owner xmlns="cb09451c-b582-4d10-a9a3-b0b7d3fa26c8">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Document_x0020_Owner>
+    <TaxCatchAll xmlns="bf46d841-c562-4023-88f4-20dc8ac77732">
+      <Value>16</Value>
+    </TaxCatchAll>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008A1C1A-9E5E-4F54-8085-06E04E5030EF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C45AD9A-5793-45F2-9DCE-DE4F0708C0D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="cb09451c-b582-4d10-a9a3-b0b7d3fa26c8"/>
+    <ds:schemaRef ds:uri="bf46d841-c562-4023-88f4-20dc8ac77732"/>
+    <ds:schemaRef ds:uri="966ee308-7f72-40a1-8e25-c38950f75702"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6681,22 +6694,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C45AD9A-5793-45F2-9DCE-DE4F0708C0D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008A1C1A-9E5E-4F54-8085-06E04E5030EF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="cb09451c-b582-4d10-a9a3-b0b7d3fa26c8"/>
-    <ds:schemaRef ds:uri="bf46d841-c562-4023-88f4-20dc8ac77732"/>
-    <ds:schemaRef ds:uri="966ee308-7f72-40a1-8e25-c38950f75702"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>